<commit_message>
added calculation in excel file
</commit_message>
<xml_diff>
--- a/DATA_EVAL/annotation_sample/results_annotation_jex6_topic5.xlsx
+++ b/DATA_EVAL/annotation_sample/results_annotation_jex6_topic5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ettor\Documents\GitHub\eurovoc_topicmodeling\DATA_EVAL\annotation_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5AE59979-BC3C-4236-BC8B-D08C68EEF2D8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2CFED066-50C3-4CF8-A7D7-D4F04275E884}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4051" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4053" uniqueCount="529">
   <si>
     <t>File name</t>
   </si>
@@ -1609,13 +1609,19 @@
   </si>
   <si>
     <t>F1</t>
+  </si>
+  <si>
+    <t>Note : très mauvais rappel en dépit du fait que le topic modeling a produit en moyenne 4.8 domaines contre 2.9 pour Jex</t>
+  </si>
+  <si>
+    <t>Note2 : le fait que certains topics ne possèdent pas de label joue également (19 topics vides sur 150)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1627,6 +1633,13 @@
       <b/>
       <sz val="16"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1652,9 +1665,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1999,8 +2013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O902"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2307,8 +2321,8 @@
         <v>526</v>
       </c>
       <c r="O15">
-        <f>(O13*O14)/(O13+O14)</f>
-        <v>7.7844311377245512E-2</v>
+        <f>2*(O13*O14)/(O13+O14)</f>
+        <v>0.15568862275449102</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -2325,7 +2339,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2360,20 +2374,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N18" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N19" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D20">
         <v>7.8997587222091186</v>
       </c>
@@ -2387,7 +2407,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D21">
         <v>21.722286118173294</v>
       </c>
@@ -2401,7 +2421,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D22">
         <v>26.666313911136303</v>
       </c>
@@ -2415,7 +2435,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D23">
         <v>7.4078719271486921</v>
       </c>
@@ -2423,7 +2443,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2458,7 +2478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>54</v>
       </c>
@@ -2469,7 +2489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>55</v>
       </c>
@@ -2480,7 +2500,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D27">
         <v>9.3383407981071258</v>
       </c>
@@ -2494,7 +2514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D28">
         <v>15.831964565741702</v>
       </c>
@@ -2508,7 +2528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D29">
         <v>20.701672258293243</v>
       </c>
@@ -2522,7 +2542,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D30">
         <v>12.189202018833953</v>
       </c>
@@ -2536,7 +2556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -2571,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>66</v>
       </c>
@@ -13806,8 +13826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179F4394-1A47-429D-BB02-4123D5AD9F97}">
   <dimension ref="A1:Q448"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14142,11 +14162,11 @@
         <v>526</v>
       </c>
       <c r="Q16">
-        <f>(rappel*précsion)/(rappel+précsion)</f>
-        <v>0.26546906187624753</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <f>2*(rappel*précsion)/(rappel+précsion)</f>
+        <v>0.53093812375249505</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -14183,8 +14203,9 @@
       <c r="L17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>54</v>
       </c>
@@ -14201,7 +14222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>55</v>
       </c>
@@ -14218,7 +14239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -14256,7 +14277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>66</v>
       </c>
@@ -14273,7 +14294,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>14</v>
       </c>
@@ -14281,7 +14302,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>63</v>
       </c>
@@ -14289,7 +14310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -14327,7 +14348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>45</v>
       </c>
@@ -14344,7 +14365,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>34</v>
       </c>
@@ -14358,7 +14379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>159</v>
       </c>
@@ -14366,17 +14387,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -14414,7 +14435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>55</v>
       </c>
@@ -14428,7 +14449,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>83</v>
       </c>

</xml_diff>